<commit_message>
Solved graph alignment problems
</commit_message>
<xml_diff>
--- a/Python/src/_Highlands/setup.xlsx
+++ b/Python/src/_Highlands/setup.xlsx
@@ -42,12 +42,6 @@
     <t>NAME</t>
   </si>
   <si>
-    <t>highlands4</t>
-  </si>
-  <si>
-    <t>survey4</t>
-  </si>
-  <si>
     <t>host</t>
   </si>
   <si>
@@ -55,6 +49,12 @@
   </si>
   <si>
     <t>OPTION</t>
+  </si>
+  <si>
+    <t>highlands5</t>
+  </si>
+  <si>
+    <t>survey2</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -467,7 +467,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -502,18 +502,18 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>9097</v>

</xml_diff>

<commit_message>
baseline before updating c3 and d3
</commit_message>
<xml_diff>
--- a/Python/src/_Highlands/setup.xlsx
+++ b/Python/src/_Highlands/setup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
     <t>highlands5</t>
   </si>
   <si>
-    <t>survey3</t>
+    <t>survey2</t>
   </si>
 </sst>
 </file>

</xml_diff>